<commit_message>
feat: menu feat: codigo refatorado
</commit_message>
<xml_diff>
--- a/motoristas.xlsx
+++ b/motoristas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayck\OneDrive\Documentos\coding\projeto openpylx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF5BAC1-5E66-495D-A227-2979F5220154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B286DAF-40BF-45EA-B869-F5EEA14242AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ESCALA OFICIAL</t>
   </si>
@@ -45,43 +45,49 @@
     <t>AJUDANTE2</t>
   </si>
   <si>
+    <t>MAYCK</t>
+  </si>
+  <si>
+    <t>DEF-1234</t>
+  </si>
+  <si>
+    <t>LAIS</t>
+  </si>
+  <si>
+    <t>ANTONY</t>
+  </si>
+  <si>
+    <t>GHI-1234</t>
+  </si>
+  <si>
+    <t>JULLIANE</t>
+  </si>
+  <si>
+    <t>QUITERIA</t>
+  </si>
+  <si>
+    <t>JKL-1234</t>
+  </si>
+  <si>
+    <t>NAYANE</t>
+  </si>
+  <si>
+    <t>CARLOS HENRIQUE</t>
+  </si>
+  <si>
+    <t>MAGGIE</t>
+  </si>
+  <si>
+    <t>JOSE CARLOS</t>
+  </si>
+  <si>
     <t>ABC-1234</t>
   </si>
   <si>
     <t>ALEX</t>
   </si>
   <si>
-    <t>JOSE CARLOS</t>
-  </si>
-  <si>
-    <t>MAYCK</t>
-  </si>
-  <si>
-    <t>DEF-1234</t>
-  </si>
-  <si>
-    <t>LAIS</t>
-  </si>
-  <si>
-    <t>ANTONY</t>
-  </si>
-  <si>
-    <t>GHI-1234</t>
-  </si>
-  <si>
-    <t>JULLIANE</t>
-  </si>
-  <si>
-    <t>QUITERIA</t>
-  </si>
-  <si>
-    <t>JKL-1234</t>
-  </si>
-  <si>
-    <t>NAYANE</t>
-  </si>
-  <si>
-    <t>CARLOS HENRIQUE</t>
+    <t>destino</t>
   </si>
 </sst>
 </file>
@@ -521,31 +527,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -556,77 +564,83 @@
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>111111</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>222222</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>333333</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>444444</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>